<commit_message>
more work on wheels configs
</commit_message>
<xml_diff>
--- a/GameData/STUCK/stockParts.xlsx
+++ b/GameData/STUCK/stockParts.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Johns Stuff\KSPDev\GameData\STUCK\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="12855"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="336">
   <si>
     <t>Part Config Path</t>
   </si>
@@ -31,9 +36,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Need to see if mask is viable for current part texture.</t>
-  </si>
-  <si>
     <t>Needs flag mesh exclude</t>
   </si>
   <si>
@@ -130,9 +132,6 @@
     <t>Squad\Parts\Aero\protectiveRocketNoseMk12\rocketNoseCone_size3.cfg</t>
   </si>
   <si>
-    <t>Squad\Parts\Aero\protectiveRocketNoseMk7\protectiveRocketNoseMk7.cfg</t>
-  </si>
-  <si>
     <t>Squad\Parts\Aero\protectiveRocketNoseMk7_v2\protectiveRocketNoseMk7_v2.cfg</t>
   </si>
   <si>
@@ -970,9 +969,6 @@
     <t>Squad\Parts\Utility\spotLightMk2\spotLightMk2.cfg</t>
   </si>
   <si>
-    <t>Squad\Parts\Utility\stackBiCoupler\stackBiCoupler.cfg</t>
-  </si>
-  <si>
     <t>Squad\Parts\Utility\stackCouplers\stackBiCoupler_v2.cfg</t>
   </si>
   <si>
@@ -982,9 +978,6 @@
     <t>Squad\Parts\Utility\stackCouplers\stackTriCoupler_v2.cfg</t>
   </si>
   <si>
-    <t>Squad\Parts\Utility\stackTriCoupler\stackTriCoupler.cfg</t>
-  </si>
-  <si>
     <t>Squad\Parts\Wheel\LandingGear\GearExtraLarge.cfg</t>
   </si>
   <si>
@@ -1015,21 +1008,9 @@
     <t>Squad\Parts\Wheel\roverWheelXL3\roverWheelXL3.cfg</t>
   </si>
   <si>
-    <t>Need normalization calculated</t>
-  </si>
-  <si>
-    <t>Need normalization calculated, Truss is extra shiny because stock texture has high gloss</t>
-  </si>
-  <si>
-    <t>LEGACY</t>
-  </si>
-  <si>
     <t>no mask exists</t>
   </si>
   <si>
-    <t>legacy part - no need to do</t>
-  </si>
-  <si>
     <t>Needs default colors set</t>
   </si>
   <si>
@@ -1037,6 +1018,15 @@
   </si>
   <si>
     <t>Mask From MWNN</t>
+  </si>
+  <si>
+    <t>Needs Shroud handled</t>
+  </si>
+  <si>
+    <t>Needs normalization data</t>
+  </si>
+  <si>
+    <t>Might need mask redo</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1360,12 +1350,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1527,9 +1511,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1575,11 +1558,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1601,9 +1587,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1627,6 +1616,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1666,16 +1662,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1690,16 +1682,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1714,9 +1702,271 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1830,6 +2080,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1878,7 +2131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1913,7 +2166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2122,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G327"/>
+  <dimension ref="A1:H324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="F317" sqref="F317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,11 +2388,12 @@
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2153,314 +2407,290 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>333</v>
-      </c>
-      <c r="G8" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>333</v>
-      </c>
-      <c r="G10" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>333</v>
-      </c>
-      <c r="G11" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>333</v>
-      </c>
-      <c r="G12" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>333</v>
-      </c>
-      <c r="G13" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>333</v>
-      </c>
-      <c r="G14" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>333</v>
-      </c>
-      <c r="G15" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
       <c r="B16" t="b">
         <v>1</v>
       </c>
@@ -2474,15 +2704,12 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>333</v>
-      </c>
-      <c r="G16" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -2497,15 +2724,12 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>333</v>
-      </c>
-      <c r="G17" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -2520,15 +2744,12 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>333</v>
-      </c>
-      <c r="G18" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -2543,15 +2764,12 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>333</v>
-      </c>
-      <c r="G19" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -2566,15 +2784,12 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>333</v>
-      </c>
-      <c r="G20" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -2589,15 +2804,12 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>333</v>
-      </c>
-      <c r="G21" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -2611,13 +2823,13 @@
       <c r="E22" t="b">
         <v>0</v>
       </c>
-      <c r="G22" t="s">
-        <v>339</v>
+      <c r="F22" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -2631,13 +2843,13 @@
       <c r="E23" t="b">
         <v>0</v>
       </c>
-      <c r="G23" t="s">
-        <v>339</v>
+      <c r="F23" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -2651,13 +2863,13 @@
       <c r="E24" t="b">
         <v>0</v>
       </c>
-      <c r="G24" t="s">
-        <v>339</v>
+      <c r="F24" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -2666,12 +2878,12 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -2680,12 +2892,12 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2694,12 +2906,12 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2708,12 +2920,12 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -2728,15 +2940,15 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="G29" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2751,15 +2963,12 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>333</v>
-      </c>
-      <c r="G30" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -2774,358 +2983,321 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>333</v>
-      </c>
-      <c r="G31" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B32" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>333</v>
-      </c>
-      <c r="G35" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>333</v>
-      </c>
-      <c r="G36" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B37" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="s">
-        <v>333</v>
-      </c>
-      <c r="G37" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>43</v>
       </c>
-      <c r="B38" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>333</v>
-      </c>
-      <c r="G38" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" t="s">
-        <v>333</v>
-      </c>
-      <c r="G39" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>45</v>
       </c>
-      <c r="B40" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" t="s">
-        <v>333</v>
-      </c>
-      <c r="G40" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>46</v>
       </c>
-      <c r="B41" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>333</v>
-      </c>
-      <c r="G41" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="B42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="s">
-        <v>333</v>
-      </c>
-      <c r="G42" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" t="b">
-        <v>1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>333</v>
-      </c>
-      <c r="G43" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>49</v>
       </c>
-      <c r="B44" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>333</v>
-      </c>
-      <c r="G44" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="s">
-        <v>333</v>
-      </c>
-      <c r="G45" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>51</v>
       </c>
-      <c r="B46" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" t="b">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>333</v>
-      </c>
-      <c r="G46" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" t="b">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>333</v>
-      </c>
-      <c r="G47" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
       <c r="B48" t="b">
         <v>0</v>
       </c>
@@ -3139,15 +3311,12 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>333</v>
-      </c>
-      <c r="G48" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" t="b">
         <v>0</v>
@@ -3162,15 +3331,12 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>333</v>
-      </c>
-      <c r="G49" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
@@ -3185,15 +3351,12 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>333</v>
-      </c>
-      <c r="G50" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" t="b">
         <v>0</v>
@@ -3208,15 +3371,12 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>333</v>
-      </c>
-      <c r="G51" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -3231,15 +3391,12 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>333</v>
-      </c>
-      <c r="G52" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -3254,15 +3411,12 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>333</v>
-      </c>
-      <c r="G53" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -3277,15 +3431,12 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>333</v>
-      </c>
-      <c r="G54" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" t="b">
         <v>0</v>
@@ -3300,15 +3451,12 @@
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>333</v>
-      </c>
-      <c r="G55" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" t="b">
         <v>0</v>
@@ -3323,15 +3471,12 @@
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>333</v>
-      </c>
-      <c r="G56" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" t="b">
         <v>0</v>
@@ -3346,15 +3491,12 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>333</v>
-      </c>
-      <c r="G57" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" t="b">
         <v>0</v>
@@ -3369,15 +3511,12 @@
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>333</v>
-      </c>
-      <c r="G58" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
@@ -3392,15 +3531,12 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>333</v>
-      </c>
-      <c r="G59" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="b">
         <v>0</v>
@@ -3415,15 +3551,12 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>333</v>
-      </c>
-      <c r="G60" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
@@ -3438,1500 +3571,1716 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>333</v>
-      </c>
-      <c r="G61" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>67</v>
-      </c>
-      <c r="B62" t="b">
-        <v>0</v>
-      </c>
-      <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>333</v>
-      </c>
-      <c r="G62" t="s">
-        <v>338</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="B63" t="b">
+        <v>0</v>
+      </c>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" t="b">
-        <v>0</v>
-      </c>
-      <c r="C64" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>6</v>
-      </c>
-      <c r="G64" t="s">
-        <v>338</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B96" t="b">
+        <v>0</v>
+      </c>
+      <c r="C96" t="b">
+        <v>1</v>
+      </c>
+      <c r="D96" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>334</v>
+      </c>
+      <c r="G96" t="s">
+        <v>330</v>
+      </c>
+      <c r="H96" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B97" t="b">
+        <v>0</v>
+      </c>
+      <c r="C97" t="b">
+        <v>1</v>
+      </c>
+      <c r="D97" t="b">
+        <v>1</v>
+      </c>
+      <c r="E97" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" t="s">
+        <v>334</v>
+      </c>
+      <c r="G97" t="s">
+        <v>330</v>
+      </c>
+      <c r="H97" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B98" t="b">
+        <v>0</v>
+      </c>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" t="s">
+        <v>334</v>
+      </c>
+      <c r="G98" t="s">
+        <v>330</v>
+      </c>
+      <c r="H98" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99" t="b">
+        <v>0</v>
+      </c>
+      <c r="C99" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>334</v>
+      </c>
+      <c r="G99" t="s">
+        <v>330</v>
+      </c>
+      <c r="H99" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B100" t="b">
+        <v>0</v>
+      </c>
+      <c r="C100" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>334</v>
+      </c>
+      <c r="G100" t="s">
+        <v>330</v>
+      </c>
+      <c r="H100" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B101" t="b">
+        <v>0</v>
+      </c>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="s">
+        <v>334</v>
+      </c>
+      <c r="G101" t="s">
+        <v>330</v>
+      </c>
+      <c r="H101" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B102" t="b">
+        <v>0</v>
+      </c>
+      <c r="C102" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>334</v>
+      </c>
+      <c r="G102" t="s">
+        <v>330</v>
+      </c>
+      <c r="H102" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B103" t="b">
+        <v>0</v>
+      </c>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" t="b">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>334</v>
+      </c>
+      <c r="G103" t="s">
+        <v>330</v>
+      </c>
+      <c r="H103" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+      <c r="G315" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
+      <c r="G316" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
+      <c r="G317" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
+      <c r="G318" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
+      <c r="G319" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
-        <v>325</v>
+      <c r="G320" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>326</v>
+        <v>325</v>
+      </c>
+      <c r="B321" t="b">
+        <v>0</v>
+      </c>
+      <c r="C321" t="b">
+        <v>1</v>
+      </c>
+      <c r="D321" t="b">
+        <v>1</v>
+      </c>
+      <c r="E321" t="b">
+        <v>1</v>
+      </c>
+      <c r="G321" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>327</v>
+        <v>326</v>
+      </c>
+      <c r="B322" t="b">
+        <v>0</v>
+      </c>
+      <c r="C322" t="b">
+        <v>1</v>
+      </c>
+      <c r="D322" t="b">
+        <v>1</v>
+      </c>
+      <c r="E322" t="b">
+        <v>1</v>
+      </c>
+      <c r="G322" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>328</v>
+        <v>327</v>
+      </c>
+      <c r="B323" t="b">
+        <v>0</v>
+      </c>
+      <c r="C323" t="b">
+        <v>1</v>
+      </c>
+      <c r="D323" t="b">
+        <v>1</v>
+      </c>
+      <c r="E323" t="b">
+        <v>1</v>
+      </c>
+      <c r="G323" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>329</v>
-      </c>
-      <c r="B324" t="b">
-        <v>0</v>
-      </c>
-      <c r="C324" t="b">
-        <v>1</v>
-      </c>
-      <c r="D324" t="b">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="G324" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B33:E33 B1:B1048576">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+  <conditionalFormatting sqref="B1:B322 B324:B1048576">
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="41" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+  <conditionalFormatting sqref="C1:C322 C324:C1048576">
+    <cfRule type="cellIs" dxfId="57" priority="36" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="25" priority="32">
+    <cfRule type="containsBlanks" dxfId="55" priority="40">
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:E2 D16:E17 D32:E34 D29:D31 D63:E63 D35:D62 D65:E1048576 D64 D22:E28">
-    <cfRule type="containsBlanks" dxfId="24" priority="25">
+  <conditionalFormatting sqref="D1:E2 D16:E17 D29:D31 D62:E62 D34:D61 D63 D22:E28 D32:E33 D64:E322 D324:E1048576">
+    <cfRule type="containsBlanks" dxfId="54" priority="33">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="34" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="35" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E15 E3:E21">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="30" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:E24">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="28" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E31">
-    <cfRule type="containsBlanks" dxfId="17" priority="16">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="46" priority="24">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="24" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E31">
-    <cfRule type="containsBlanks" dxfId="14" priority="13">
+    <cfRule type="containsBlanks" dxfId="44" priority="21">
       <formula>LEN(TRIM(E29))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:E62">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
-      <formula>LEN(TRIM(E35))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+  <conditionalFormatting sqref="E34:E61">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="containsBlanks" dxfId="40" priority="18">
+      <formula>LEN(TRIM(E34))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="18" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:E62">
-    <cfRule type="containsBlanks" dxfId="8" priority="7">
-      <formula>LEN(TRIM(E35))=0</formula>
+  <conditionalFormatting sqref="E34:E61">
+    <cfRule type="containsBlanks" dxfId="38" priority="15">
+      <formula>LEN(TRIM(E34))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
-      <formula>LEN(TRIM(E64))=0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+  <conditionalFormatting sqref="E63">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="containsBlanks" dxfId="34" priority="12">
+      <formula>LEN(TRIM(E63))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
-      <formula>LEN(TRIM(E64))=0</formula>
+  <conditionalFormatting sqref="E63">
+    <cfRule type="containsBlanks" dxfId="32" priority="9">
+      <formula>LEN(TRIM(E63))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B323">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C323">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="9" priority="-1">
+      <formula>LEN(TRIM(C323))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D323:E323">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(D323))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
more work on things...
</commit_message>
<xml_diff>
--- a/GameData/STUCK/stockParts.xlsx
+++ b/GameData/STUCK/stockParts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Johns Stuff\KSPDev\GameData\STUCK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_source\STUCK\GameData\STUCK\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1510,223 +1510,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2057,8 +1841,8 @@
   <dimension ref="A1:K305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5166,7 +4950,7 @@
         <v>1</v>
       </c>
       <c r="D117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117" t="b">
         <v>1</v>
@@ -5192,7 +4976,7 @@
         <v>1</v>
       </c>
       <c r="D118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E118" t="b">
         <v>1</v>
@@ -5218,7 +5002,7 @@
         <v>1</v>
       </c>
       <c r="D119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119" t="b">
         <v>1</v>
@@ -5244,7 +5028,7 @@
         <v>1</v>
       </c>
       <c r="D120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120" t="b">
         <v>1</v>
@@ -5270,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="D121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
more masking work -- add mask for rockomax adapters (need configs; uses variant system) * Small nosecone mask could use work -- currently using very simple single-color masking
</commit_message>
<xml_diff>
--- a/GameData/STUCK/stockParts.xlsx
+++ b/GameData/STUCK/stockParts.xlsx
@@ -1842,7 +1842,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="J1" t="str">
         <f>"MASKS: " &amp; COUNTIF(B2:B350, TRUE)</f>
-        <v>MASKS: 204</v>
+        <v>MASKS: 205</v>
       </c>
       <c r="K1" t="str">
         <f>"TOTAL:" &amp; COUNTIF(A2:A350, "&gt;""")</f>
@@ -1900,7 +1900,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>

</xml_diff>